<commit_message>
Replaced bad data with good data.
</commit_message>
<xml_diff>
--- a/preproc/PilotAges.xlsx
+++ b/preproc/PilotAges.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Calvin\Desktop\worb\SocioSpacial\preproc\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5A558828-A68C-485A-BD19-BAABF770B217}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{DB305D61-FF2E-43CF-8EB1-0FDF65BC9936}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -48,7 +42,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -58,12 +52,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -78,8 +78,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -140,7 +141,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -192,7 +193,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -386,23 +387,23 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DFA944B-99C8-4D6F-AF03-8AD9C6F046E2}">
-  <dimension ref="A1:B17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B17"/>
+      <selection activeCell="C1" sqref="C1:D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -410,124 +411,138 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>